<commit_message>
Update network description for transportation model network
</commit_message>
<xml_diff>
--- a/Transportation/data/Transportation.xlsx
+++ b/Transportation/data/Transportation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Adam_Project\GAMS_Code\Transportation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Apps\demos\Transportation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="11580" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="3" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>0.8</t>
   </si>
   <si>
-    <t>Gas Transmission Problem - Belgium</t>
-  </si>
-  <si>
     <t>Resource</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>shipment_quantities</t>
+  </si>
+  <si>
+    <t>Network and scenario data for transportation model</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -622,7 +624,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -658,25 +660,25 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -684,27 +686,27 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -727,119 +729,119 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
       <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
       <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="K6" t="s">
-        <v>32</v>
-      </c>
       <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
         <v>31</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -880,16 +882,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -897,18 +899,18 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -922,65 +924,65 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
       <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1043,15 +1045,15 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>-13387679</v>
@@ -1060,7 +1062,7 @@
         <v>4203113</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1">
         <v>160</v>
@@ -1068,7 +1070,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>-13733973</v>
@@ -1077,7 +1079,7 @@
         <v>4921749</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1">
         <v>85</v>
@@ -1085,7 +1087,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>-13650204</v>
@@ -1094,7 +1096,7 @@
         <v>5864680</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1">
         <v>320</v>
@@ -1102,7 +1104,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>-9753849</v>
@@ -1111,7 +1113,7 @@
         <v>5143421</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1">
         <v>39</v>
@@ -1119,7 +1121,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>-9088808</v>
@@ -1128,7 +1130,7 @@
         <v>5089941</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1">
         <v>28</v>
@@ -1136,7 +1138,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>-9244019</v>
@@ -1145,7 +1147,7 @@
         <v>5214220</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1">
         <v>42</v>
@@ -1153,7 +1155,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>-9786083</v>
@@ -1162,7 +1164,7 @@
         <v>5319729</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1">
         <v>25</v>
@@ -1170,7 +1172,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>-10381301</v>
@@ -1179,7 +1181,7 @@
         <v>5618890</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1">
         <v>55</v>
@@ -1187,7 +1189,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>-8231842</v>
@@ -1196,7 +1198,7 @@
         <v>4972068</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1">
         <v>70</v>
@@ -1244,10 +1246,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -1256,7 +1258,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1267,21 +1269,21 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1">
         <v>9.1</v>
@@ -1292,16 +1294,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1">
         <v>14.3</v>
@@ -1312,16 +1314,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1">
         <v>12.5</v>
@@ -1332,16 +1334,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1">
         <v>15.55</v>
@@ -1352,16 +1354,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1">
         <v>13.8</v>
@@ -1372,16 +1374,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1">
         <v>10.8</v>
@@ -1392,16 +1394,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1">
         <v>15.6</v>
@@ -1412,16 +1414,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1">
         <v>17.100000000000001</v>
@@ -1432,16 +1434,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="1">
         <v>13.2</v>
@@ -1452,16 +1454,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1">
         <v>13.4</v>
@@ -1472,16 +1474,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="1">
         <v>12.8</v>
@@ -1492,16 +1494,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1">
         <v>13.2</v>
@@ -1512,16 +1514,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1">
         <v>14.6</v>
@@ -1532,16 +1534,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="1">
         <v>13.9</v>
@@ -1552,16 +1554,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1">
         <v>13.4</v>
@@ -1572,16 +1574,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1">
         <v>15.2</v>
@@ -1592,16 +1594,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1">
         <v>13.6</v>
@@ -1612,16 +1614,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1">
         <v>14.4</v>
@@ -1743,7 +1745,7 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1825,7 +1827,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1872,10 +1874,10 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1907,319 +1909,319 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2296,61 +2298,61 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
@@ -2358,63 +2360,63 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AD2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AH2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AJ2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -2473,335 +2475,335 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s">
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R4" t="s">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T4" t="s">
         <v>0</v>
       </c>
       <c r="U4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V4" t="s">
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X4" t="s">
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z4" t="s">
         <v>0</v>
       </c>
       <c r="AA4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB4" t="s">
         <v>0</v>
       </c>
       <c r="AC4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AD4" t="s">
         <v>0</v>
       </c>
       <c r="AE4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AF4" t="s">
         <v>0</v>
       </c>
       <c r="AG4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH4" t="s">
         <v>0</v>
       </c>
       <c r="AI4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AJ4" t="s">
         <v>0</v>
       </c>
       <c r="AK4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Z5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AB5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AD5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AE5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AF5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AG5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AH5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AI5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AJ5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AK5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
       <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
       <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="K6" t="s">
-        <v>32</v>
-      </c>
       <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
       <c r="N6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" t="s">
         <v>31</v>
       </c>
-      <c r="O6" t="s">
-        <v>32</v>
-      </c>
       <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" t="s">
-        <v>32</v>
-      </c>
       <c r="R6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" t="s">
         <v>31</v>
       </c>
-      <c r="S6" t="s">
-        <v>32</v>
-      </c>
       <c r="T6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U6" t="s">
         <v>31</v>
       </c>
-      <c r="U6" t="s">
-        <v>32</v>
-      </c>
       <c r="V6" t="s">
+        <v>30</v>
+      </c>
+      <c r="W6" t="s">
         <v>31</v>
       </c>
-      <c r="W6" t="s">
-        <v>32</v>
-      </c>
       <c r="X6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y6" t="s">
         <v>31</v>
       </c>
-      <c r="Y6" t="s">
-        <v>32</v>
-      </c>
       <c r="Z6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="s">
         <v>31</v>
       </c>
-      <c r="AA6" t="s">
-        <v>32</v>
-      </c>
       <c r="AB6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC6" t="s">
         <v>31</v>
       </c>
-      <c r="AC6" t="s">
-        <v>32</v>
-      </c>
       <c r="AD6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE6" t="s">
         <v>31</v>
       </c>
-      <c r="AE6" t="s">
-        <v>32</v>
-      </c>
       <c r="AF6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG6" t="s">
         <v>31</v>
       </c>
-      <c r="AG6" t="s">
-        <v>32</v>
-      </c>
       <c r="AH6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI6" t="s">
         <v>31</v>
       </c>
-      <c r="AI6" t="s">
-        <v>32</v>
-      </c>
       <c r="AJ6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK6" t="s">
         <v>31</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>